<commit_message>
Game logic 99% done
</commit_message>
<xml_diff>
--- a/Copy of Team Project Tracking Sheets.xlsx
+++ b/Copy of Team Project Tracking Sheets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ty9253er\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yb5243yv\Dropbox\Workspace - Java - 2017-2018\Card Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>Copyright - Sudharsan Iyengar - August 2017.</t>
   </si>
@@ -139,6 +139,48 @@
   </si>
   <si>
     <t>4 hr</t>
+  </si>
+  <si>
+    <t>Jared DuPont</t>
+  </si>
+  <si>
+    <t>6hr</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Client GUI</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Server GUI</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>1hr</t>
+  </si>
+  <si>
+    <t>5hr</t>
+  </si>
+  <si>
+    <t>Communicate and get updates from server</t>
+  </si>
+  <si>
+    <t>Display info and get player choices</t>
+  </si>
+  <si>
+    <t>Handle game logic and client communication</t>
+  </si>
+  <si>
+    <t>Jared</t>
+  </si>
+  <si>
+    <t>Display server info, very basic</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1114,7 @@
   <dimension ref="B1:M16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,8 +1220,12 @@
       <c r="J8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
+      <c r="L8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
@@ -1206,7 +1252,9 @@
       <c r="J10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="11"/>
+      <c r="L10" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="M10" s="11"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -1228,10 +1276,18 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="I12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
@@ -1254,8 +1310,12 @@
       <c r="G14" s="8"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
+      <c r="L14" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
@@ -1290,13 +1350,13 @@
   <dimension ref="B3:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="47" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1317,24 +1377,46 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="B7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="D8" s="14"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="B9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
+      <c r="B10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
@@ -1417,7 +1499,7 @@
   <dimension ref="C2:I26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1832,7 +1914,7 @@
   <dimension ref="C3:G27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>